<commit_message>
Updated existing student error in validation/migration scripts
</commit_message>
<xml_diff>
--- a/data/epas333.xlsx
+++ b/data/epas333.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t xml:space="preserve">ΤΜΗΜΑ ΕΙΣΑΓΩΓΗΣ</t>
   </si>
@@ -197,9 +197,6 @@
   </si>
   <si>
     <t xml:space="preserve">ΝΑΙ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">er</t>
   </si>
   <si>
     <t xml:space="preserve">28/07/2025</t>
@@ -743,17 +740,17 @@
       <c r="AF2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AG2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="AH2" s="10" t="s">
+      <c r="AI2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="AI2" s="2" t="s">
+      <c r="AJ2" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="AJ2" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="AK2" s="1" t="n">
         <v>10.5</v>

</xml_diff>